<commit_message>
Made various bug fixes, added a new format option, and modified the sample .xlsx file.
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyler\Desktop\Scripts\DataGenerator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tph19\Projects\DataGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69FD1A4A-B743-4CCF-8BC9-13500A473663}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CustomerTB" sheetId="1" r:id="rId1"/>
-    <sheet name="Product_Table" sheetId="2" r:id="rId2"/>
+    <sheet name="ContactTB" sheetId="3" r:id="rId2"/>
+    <sheet name="ProductTb" sheetId="5" r:id="rId3"/>
+    <sheet name="OrderTB" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,42 +28,81 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
-  <si>
-    <t>cust_name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>cust_id</t>
   </si>
   <si>
-    <t>cust_add</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
-    <t>transaction_id</t>
-  </si>
-  <si>
     <t>[A-Z]{4}[0-9]{4}</t>
   </si>
   <si>
-    <t>product_code</t>
-  </si>
-  <si>
-    <t>[A-Z]{8}</t>
-  </si>
-  <si>
     <t>{{primary_address}}</t>
   </si>
   <si>
-    <t>{{first_name}} {{last_name}}</t>
+    <t>cust_first</t>
+  </si>
+  <si>
+    <t>cust_last</t>
+  </si>
+  <si>
+    <t>{{last_name}}</t>
+  </si>
+  <si>
+    <t>{{first_name}}</t>
+  </si>
+  <si>
+    <t>first</t>
+  </si>
+  <si>
+    <t>last</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>{{email}}</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>order_id</t>
+  </si>
+  <si>
+    <t>[A-Z]{5}[0-9]{4}</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>[1.00-100.00]</t>
+  </si>
+  <si>
+    <t>customer_id</t>
+  </si>
+  <si>
+    <t>[0-9]{3}-[0-9]{3}-[0-9]{4}</t>
+  </si>
+  <si>
+    <t>{{alphanum}}{10}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -371,81 +413,186 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="137" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69869DFD-BA05-4E11-9B3B-1C27DA8C661E}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView zoomScale="145" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BB26782-71A7-4DD1-8026-3D9FD2D3C190}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView zoomScale="159" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ED52796-DC43-4B96-9EEB-DCFEA1BEC61E}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="155" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added date generation function Updated README.md Fixed a capitalization error in tables.xlsx
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tph19\Projects\DataGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69FD1A4A-B743-4CCF-8BC9-13500A473663}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1733ACC5-75EF-4EBC-A556-1E6FC853F4DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CustomerTB" sheetId="1" r:id="rId1"/>
     <sheet name="ContactTB" sheetId="3" r:id="rId2"/>
-    <sheet name="ProductTb" sheetId="5" r:id="rId3"/>
+    <sheet name="ProductTB" sheetId="5" r:id="rId3"/>
     <sheet name="OrderTB" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
@@ -532,7 +532,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BB26782-71A7-4DD1-8026-3D9FD2D3C190}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView zoomScale="159" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="159" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -566,7 +566,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ED52796-DC43-4B96-9EEB-DCFEA1BEC61E}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="155" workbookViewId="0">
+    <sheetView zoomScale="155" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>